<commit_message>
No changes were provided to summarize.
</commit_message>
<xml_diff>
--- a/AI-driven-Project-Management-main/案件/横須賀地方隊/概算見積もり_横須賀地方隊_オフィシャルサイト新規制作.xlsx
+++ b/AI-driven-Project-Management-main/案件/横須賀地方隊/概算見積もり_横須賀地方隊_オフィシャルサイト新規制作.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tomokazu.tateishi/Documents/PM/AI-driven-Project-Management-main/案件/横須賀地方隊/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D4D22806-D23F-B346-AD0A-AB8C116037A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C9BC2BB-E1B5-2D4F-9968-85ABA1E6CFA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-31200" yWindow="-21100" windowWidth="38400" windowHeight="21100" activeTab="2" xr2:uid="{EFFAFE3D-F5E4-7145-AD16-DAFC9F1FB8C0}"/>
+    <workbookView xWindow="-31200" yWindow="-21100" windowWidth="38400" windowHeight="19860" activeTab="1" xr2:uid="{EFFAFE3D-F5E4-7145-AD16-DAFC9F1FB8C0}"/>
   </bookViews>
   <sheets>
     <sheet name="提示用" sheetId="10" r:id="rId1"/>
     <sheet name="見積" sheetId="5" r:id="rId2"/>
     <sheet name="工数" sheetId="9" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="12" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="77">
   <si>
     <t>役割</t>
   </si>
@@ -53,12 +54,6 @@
   </si>
   <si>
     <t>一式</t>
-  </si>
-  <si>
-    <t>貼り付け時マージン</t>
-  </si>
-  <si>
-    <t>設計書兼マニュアル資料作成</t>
   </si>
   <si>
     <t>単価計算</t>
@@ -168,10 +163,7 @@
     <t>(税込)</t>
   </si>
   <si>
-    <t xml:space="preserve">yokosukatihousoukanbu </t>
-  </si>
-  <si>
-    <t>横須賀地方総監部</t>
+    <t>デザイナー</t>
   </si>
   <si>
     <t>デザイナー</t>
@@ -190,6 +182,151 @@
       <t xml:space="preserve">ガツ </t>
     </rPh>
     <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デザイン</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>MTG</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>下層ページワイヤー</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">カソウページ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>TOPページワイヤー</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実装チェック</t>
+    <rPh sb="0" eb="2">
+      <t xml:space="preserve">ジッソウチェック </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ブラウザ確認</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>デザインFB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>作業内容</t>
+  </si>
+  <si>
+    <t>作業内容</t>
+    <rPh sb="0" eb="4">
+      <t xml:space="preserve">サギョウナイヨウ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ワイヤーFB</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>実装フォロー</t>
+    <rPh sb="0" eb="1">
+      <t xml:space="preserve">ジッソウ </t>
+    </rPh>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>案件名</t>
+  </si>
+  <si>
+    <t>横須賀地方総監部オフィシャルサイト新規制作</t>
+  </si>
+  <si>
+    <t>案件概要</t>
+  </si>
+  <si>
+    <t>海上自衛隊横須賀地方総監部のオフィシャルサイト新規制作（5P）案件です。</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://www.mod.go.jp/msdf/yokosuka/index.html</t>
+  </si>
+  <si>
+    <t>作業期間</t>
+  </si>
+  <si>
+    <t>契約決定日: 令和8年2月13日（予定）</t>
+  </si>
+  <si>
+    <t>納期: 令和8年3月13日</t>
+  </si>
+  <si>
+    <t>実作業期間: 約1週間</t>
+  </si>
+  <si>
+    <t>【制作ページ（全5ページ）】</t>
+  </si>
+  <si>
+    <t>トップページ（問い合わせフォーム含む）</t>
+  </si>
+  <si>
+    <t>総監の経歴（バイオ）ページ</t>
+  </si>
+  <si>
+    <t>採用情報ページ（PDFリンク）</t>
+  </si>
+  <si>
+    <t>年間行事ページ（写真付き、年度別表示）</t>
+  </si>
+  <si>
+    <t>部隊紹介ページ</t>
+  </si>
+  <si>
+    <t>【技術要件】</t>
+  </si>
+  <si>
+    <t>レスポンシブデザイン（スマートフォン対応必須）</t>
+  </si>
+  <si>
+    <t>CSS/HTMLファイルで納品</t>
+  </si>
+  <si>
+    <t>ブラウザチェック（Chrome、Firefox、Safari、Edge等の主要ブラウザ対応確認）：最新バージョン</t>
+  </si>
+  <si>
+    <t>【制作フロー】</t>
+  </si>
+  <si>
+    <t>官側からデザイン素案の提供を受領</t>
+  </si>
+  <si>
+    <t>版下（レイアウト案）を提示</t>
+  </si>
+  <si>
+    <t>官側の校正を受ける</t>
+  </si>
+  <si>
+    <t>本制作</t>
+  </si>
+  <si>
+    <t>完成検査・受領検査</t>
+  </si>
+  <si>
+    <t>【その他】</t>
+  </si>
+  <si>
+    <t>リモート作業可</t>
+  </si>
+  <si>
+    <t>（ヘッダー等を）下層ページとの整合性を合わせる必要はなし</t>
+  </si>
+  <si>
+    <t>納品後1年間の不具合補償が必要</t>
   </si>
 </sst>
 </file>
@@ -201,7 +338,7 @@
     <numFmt numFmtId="177" formatCode="0.00_);[Red]\(0.00\)"/>
     <numFmt numFmtId="178" formatCode="&quot;¥&quot;#,##0_);[Red]\(&quot;¥&quot;#,##0\)"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="16">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -311,6 +448,15 @@
       <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="メイリオ"/>
+      <family val="2"/>
+      <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="メイリオ"/>
+      <family val="2"/>
       <charset val="128"/>
     </font>
   </fonts>
@@ -364,7 +510,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="25">
     <border>
       <left/>
       <right/>
@@ -583,6 +729,139 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
@@ -592,7 +871,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -742,6 +1021,42 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1073,10 +1388,10 @@
   <sheetPr>
     <tabColor rgb="FFFF0000"/>
   </sheetPr>
-  <dimension ref="B3:F6"/>
+  <dimension ref="B3:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="20"/>
@@ -1086,7 +1401,7 @@
     <col min="4" max="4" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:6" ht="23">
+    <row r="3" spans="2:4" ht="23">
       <c r="B3" s="3" t="s">
         <v>0</v>
       </c>
@@ -1097,7 +1412,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="23">
+    <row r="4" spans="2:4" ht="23">
       <c r="B4" s="43" t="s">
         <v>3</v>
       </c>
@@ -1105,26 +1420,34 @@
         <v>4</v>
       </c>
       <c r="D4" s="19">
-        <v>160000</v>
-      </c>
-      <c r="F4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" ht="23">
-      <c r="B5" s="43" t="s">
-        <v>6</v>
+        <v>780000.00000000012</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4" ht="23">
+      <c r="B5" s="50" t="s">
+        <v>36</v>
       </c>
       <c r="C5" s="45" t="s">
         <v>4</v>
       </c>
       <c r="D5" s="46">
-        <v>412500</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" ht="23">
-      <c r="D6" s="47">
-        <v>572500</v>
+        <v>480000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4" ht="23">
+      <c r="B6" s="50" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="46">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="23">
+      <c r="D7" s="47">
+        <v>1760000</v>
       </c>
     </row>
   </sheetData>
@@ -1137,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9E1A0ADB-3264-4741-BBE4-3E3882337450}">
   <dimension ref="B2:U109"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:D5"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="19.5" customHeight="1"/>
@@ -1170,7 +1493,7 @@
   <sheetData>
     <row r="2" spans="2:21" ht="32" customHeight="1">
       <c r="B2" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -1186,115 +1509,115 @@
         <v>0</v>
       </c>
       <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="F3" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="G3" s="17" t="s">
         <v>10</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="17" t="s">
-        <v>12</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="M3" s="1"/>
+    </row>
+    <row r="4" spans="2:21" ht="24" thickBot="1">
+      <c r="B4" s="5" t="s">
         <v>15</v>
-      </c>
-      <c r="L3" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="M3" s="1"/>
-    </row>
-    <row r="4" spans="2:21" ht="23">
-      <c r="B4" s="5" t="s">
-        <v>17</v>
       </c>
       <c r="C4" s="35">
         <v>800000</v>
       </c>
       <c r="D4" s="35">
-        <v>1600000</v>
+        <v>1300000</v>
       </c>
       <c r="E4" s="36">
-        <v>0.1</v>
+        <v>0.60000000000000009</v>
       </c>
       <c r="F4" s="19">
         <f>C4*E4</f>
-        <v>80000</v>
+        <v>480000.00000000006</v>
       </c>
       <c r="G4" s="19">
         <f>D4*E4</f>
-        <v>160000</v>
+        <v>780000.00000000012</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="I4" s="12">
         <v>0.1</v>
       </c>
       <c r="J4" s="13">
-        <f>ROUNDUP(F6/(1-I4),-4)</f>
-        <v>370000</v>
+        <f>ROUNDUP(F7/(1-I4),-4)</f>
+        <v>1160000</v>
       </c>
       <c r="K4" s="14">
-        <f>J4-F6</f>
-        <v>40000</v>
+        <f>J4-F7</f>
+        <v>120000</v>
       </c>
       <c r="L4" s="13">
         <f>J4*1.1</f>
-        <v>407000.00000000006</v>
+        <v>1276000</v>
       </c>
       <c r="M4" s="1"/>
       <c r="R4" s="26"/>
     </row>
-    <row r="5" spans="2:21" ht="23">
-      <c r="B5" s="25" t="s">
-        <v>19</v>
+    <row r="5" spans="2:21" ht="24" thickBot="1">
+      <c r="B5" s="5" t="s">
+        <v>15</v>
       </c>
       <c r="C5" s="35">
-        <v>1000000</v>
+        <v>650000</v>
       </c>
       <c r="D5" s="35">
-        <v>1650000</v>
+        <v>1200000</v>
       </c>
       <c r="E5" s="36">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="F5" s="19">
         <f>C5*E5</f>
-        <v>250000</v>
+        <v>260000</v>
       </c>
       <c r="G5" s="19">
         <f>D5*E5</f>
-        <v>412500</v>
+        <v>480000</v>
       </c>
       <c r="H5" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="I5" s="12">
         <v>0.15</v>
       </c>
       <c r="J5" s="13">
-        <f>ROUNDUP(F6/(1-I5),-4)</f>
-        <v>390000</v>
+        <f>ROUNDUP(F7/(1-I5),-4)</f>
+        <v>1230000</v>
       </c>
       <c r="K5" s="14">
-        <f>J5-F6</f>
-        <v>60000</v>
+        <f>J5-F7</f>
+        <v>190000</v>
       </c>
       <c r="L5" s="13">
         <f t="shared" ref="L5:L7" si="0">J5*1.1</f>
-        <v>429000.00000000006</v>
+        <v>1353000</v>
       </c>
       <c r="M5" s="1"/>
       <c r="Q5" s="28"/>
@@ -1302,37 +1625,42 @@
       <c r="S5" s="27"/>
       <c r="T5" s="27"/>
     </row>
-    <row r="6" spans="2:21" ht="21.75" customHeight="1">
-      <c r="D6" s="41" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="42">
-        <f>SUM(E4:E5)</f>
-        <v>0.35</v>
-      </c>
-      <c r="F6" s="20">
-        <f>SUM(F4:F5)</f>
-        <v>330000</v>
-      </c>
-      <c r="G6" s="20">
-        <f>SUM(G4:G5)</f>
-        <v>572500</v>
+    <row r="6" spans="2:21" ht="21.75" customHeight="1" thickBot="1">
+      <c r="B6" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="35">
+        <v>300000</v>
+      </c>
+      <c r="D6" s="35">
+        <v>500000</v>
+      </c>
+      <c r="E6" s="36">
+        <v>1</v>
+      </c>
+      <c r="F6" s="19">
+        <f>C6*E6</f>
+        <v>300000</v>
+      </c>
+      <c r="G6" s="19">
+        <f>D6*E6</f>
+        <v>500000</v>
       </c>
       <c r="H6" s="1"/>
       <c r="I6" s="12">
         <v>0.2</v>
       </c>
       <c r="J6" s="13">
-        <f>ROUNDUP(F6/(1-I6),-4)</f>
-        <v>420000</v>
+        <f>ROUNDUP(F7/(1-I6),-4)</f>
+        <v>1300000</v>
       </c>
       <c r="K6" s="14">
-        <f>J6-F6</f>
-        <v>90000</v>
+        <f>J6-F7</f>
+        <v>260000</v>
       </c>
       <c r="L6" s="13">
         <f t="shared" si="0"/>
-        <v>462000.00000000006</v>
+        <v>1430000</v>
       </c>
       <c r="M6" s="1"/>
       <c r="Q6" s="28"/>
@@ -1341,24 +1669,37 @@
       <c r="T6" s="27"/>
       <c r="U6" s="27"/>
     </row>
-    <row r="7" spans="2:21" ht="21.75" customHeight="1">
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+    <row r="7" spans="2:21" ht="21.75" customHeight="1" thickTop="1">
+      <c r="D7" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="42">
+        <f>SUM(E4:E6)</f>
+        <v>2</v>
+      </c>
+      <c r="F7" s="20">
+        <f>SUM(F4:F6)</f>
+        <v>1040000</v>
+      </c>
+      <c r="G7" s="20">
+        <f>SUM(G4:G6)</f>
+        <v>1760000</v>
+      </c>
       <c r="H7" s="1"/>
       <c r="I7" s="12">
         <v>0.25</v>
       </c>
       <c r="J7" s="13">
-        <f>ROUNDUP(F6/(1-I7),-4)</f>
-        <v>440000</v>
+        <f>ROUNDUP(F7/(1-I7),-4)</f>
+        <v>1390000</v>
       </c>
       <c r="K7" s="14">
-        <f>J7-F6</f>
-        <v>110000</v>
+        <f>J7-F7</f>
+        <v>350000</v>
       </c>
       <c r="L7" s="13">
         <f t="shared" si="0"/>
-        <v>484000.00000000006</v>
+        <v>1529000.0000000002</v>
       </c>
       <c r="M7" s="1"/>
       <c r="Q7" s="28"/>
@@ -1368,29 +1709,23 @@
       <c r="U7" s="27"/>
     </row>
     <row r="8" spans="2:21" ht="22" customHeight="1">
-      <c r="E8" s="29" t="s">
-        <v>22</v>
-      </c>
-      <c r="F8" s="21">
-        <f>G6</f>
-        <v>572500</v>
-      </c>
+      <c r="F8" s="1"/>
       <c r="G8" s="1"/>
       <c r="H8" s="1"/>
       <c r="I8" s="12">
         <v>0.3</v>
       </c>
       <c r="J8" s="13">
-        <f>ROUNDUP(F6/(1-I8),-4)</f>
-        <v>480000</v>
+        <f>ROUNDUP(F7/(1-I8),-4)</f>
+        <v>1490000</v>
       </c>
       <c r="K8" s="14">
-        <f>J8-F6</f>
-        <v>150000</v>
+        <f>J8-F7</f>
+        <v>450000</v>
       </c>
       <c r="L8" s="13">
         <f>J8*1.1</f>
-        <v>528000</v>
+        <v>1639000.0000000002</v>
       </c>
       <c r="M8" s="1"/>
       <c r="Q8" s="28"/>
@@ -1400,13 +1735,12 @@
       <c r="U8" s="27"/>
     </row>
     <row r="9" spans="2:21" ht="21.75" customHeight="1">
-      <c r="B9" s="9"/>
-      <c r="E9" s="30" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" s="22">
-        <f>G6-F6</f>
-        <v>242500</v>
+      <c r="E9" s="29" t="s">
+        <v>20</v>
+      </c>
+      <c r="F9" s="21">
+        <f>G7</f>
+        <v>1760000</v>
       </c>
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
@@ -1414,16 +1748,16 @@
         <v>0.35</v>
       </c>
       <c r="J9" s="13">
-        <f>ROUNDUP(F6/(1-I9),-4)</f>
-        <v>510000</v>
+        <f>ROUNDUP(F7/(1-I9),-4)</f>
+        <v>1600000</v>
       </c>
       <c r="K9" s="14">
-        <f>J9-F6</f>
-        <v>180000</v>
+        <f>J9-F7</f>
+        <v>560000</v>
       </c>
       <c r="L9" s="13">
         <f>J9*1.1</f>
-        <v>561000</v>
+        <v>1760000.0000000002</v>
       </c>
       <c r="M9" s="1"/>
       <c r="Q9" s="28"/>
@@ -1433,13 +1767,13 @@
       <c r="U9" s="27"/>
     </row>
     <row r="10" spans="2:21" ht="19.5" customHeight="1">
-      <c r="D10" s="15"/>
-      <c r="E10" s="31" t="s">
-        <v>24</v>
-      </c>
-      <c r="F10" s="23">
-        <f>F6</f>
-        <v>330000</v>
+      <c r="B10" s="9"/>
+      <c r="E10" s="30" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="22">
+        <f>G7-F7</f>
+        <v>720000</v>
       </c>
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
@@ -1447,16 +1781,16 @@
         <v>0.4</v>
       </c>
       <c r="J10" s="13">
-        <f>ROUNDUP(F6/(1-I10),-4)</f>
-        <v>550000</v>
+        <f>ROUNDUP(F7/(1-I10),-4)</f>
+        <v>1740000</v>
       </c>
       <c r="K10" s="14">
-        <f>J10-F6</f>
-        <v>220000</v>
+        <f>J10-F7</f>
+        <v>700000</v>
       </c>
       <c r="L10" s="13">
         <f>J10*1.1</f>
-        <v>605000</v>
+        <v>1914000.0000000002</v>
       </c>
       <c r="M10" s="1"/>
       <c r="Q10" s="28"/>
@@ -1468,28 +1802,28 @@
     <row r="11" spans="2:21" ht="21.75" customHeight="1">
       <c r="D11" s="15"/>
       <c r="E11" s="31" t="s">
-        <v>13</v>
-      </c>
-      <c r="F11" s="16">
-        <f>F9/F8</f>
-        <v>0.42358078602620086</v>
-      </c>
-      <c r="G11" s="15"/>
+        <v>22</v>
+      </c>
+      <c r="F11" s="23">
+        <f>F7</f>
+        <v>1040000</v>
+      </c>
+      <c r="G11" s="1"/>
       <c r="H11" s="1"/>
       <c r="I11" s="12">
         <v>0.45</v>
       </c>
       <c r="J11" s="13">
-        <f>ROUNDUP(F6/(1-I11),-4)</f>
-        <v>600000</v>
+        <f>ROUNDUP(F7/(1-I11),-4)</f>
+        <v>1900000</v>
       </c>
       <c r="K11" s="14">
-        <f>J11-F6</f>
-        <v>270000</v>
+        <f>J11-F7</f>
+        <v>860000</v>
       </c>
       <c r="L11" s="13">
         <f>J11*1.1</f>
-        <v>660000</v>
+        <v>2090000.0000000002</v>
       </c>
       <c r="M11" s="1"/>
       <c r="Q11" s="28"/>
@@ -1499,8 +1833,15 @@
       <c r="U11" s="27"/>
     </row>
     <row r="12" spans="2:21" ht="29" customHeight="1">
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="D12" s="15"/>
+      <c r="E12" s="31" t="s">
+        <v>11</v>
+      </c>
+      <c r="F12" s="16">
+        <f>F10/F9</f>
+        <v>0.40909090909090912</v>
+      </c>
+      <c r="G12" s="15"/>
       <c r="H12" s="15"/>
       <c r="I12" s="1"/>
       <c r="J12" s="8"/>
@@ -1549,22 +1890,102 @@
       <c r="L16" s="1"/>
       <c r="M16" s="1"/>
     </row>
-    <row r="17" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="18" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="19" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="20" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="21" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="22" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="23" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="24" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="25" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="26" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="27" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="28" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="29" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="30" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="31" s="1" customFormat="1" ht="19.5" customHeight="1"/>
-    <row r="32" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="17" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="18" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="19" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="20" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="21" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B21" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E21" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="G21" s="17" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B22" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C22" s="35">
+        <v>800000</v>
+      </c>
+      <c r="D22" s="35">
+        <v>1300000</v>
+      </c>
+      <c r="E22" s="36">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="19">
+        <f>C22*E22</f>
+        <v>160000</v>
+      </c>
+      <c r="G22" s="19">
+        <f>D22*E22</f>
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B23" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C23" s="35"/>
+      <c r="D23" s="35"/>
+      <c r="E23" s="36"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19">
+        <f>D23*E23</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1">
+      <c r="B24" s="25" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="19"/>
+      <c r="G24" s="19">
+        <f>D24*E24</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1" thickTop="1">
+      <c r="D25" s="41" t="s">
+        <v>19</v>
+      </c>
+      <c r="E25" s="42">
+        <f>SUM(E22:E24)</f>
+        <v>0.2</v>
+      </c>
+      <c r="F25" s="20">
+        <f>SUM(F22:F24)</f>
+        <v>160000</v>
+      </c>
+      <c r="G25" s="20">
+        <f>SUM(G22:G24)</f>
+        <v>260000</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="27" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="28" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="29" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="30" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="31" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
+    <row r="32" spans="2:7" s="1" customFormat="1" ht="19.5" customHeight="1"/>
     <row r="33" s="1" customFormat="1" ht="19.5" customHeight="1"/>
     <row r="34" s="1" customFormat="1" ht="19.5" customHeight="1"/>
     <row r="35" s="1" customFormat="1" ht="19.5" customHeight="1"/>
@@ -1652,8 +2073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B61685A-0B46-41A9-AF67-C5940DA57554}">
   <dimension ref="B2:T99"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N36" sqref="N36"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C28" sqref="C28:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="19.5" customHeight="1"/>
@@ -1684,62 +2105,62 @@
     </row>
     <row r="3" spans="2:20" ht="24.75" customHeight="1">
       <c r="B3" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="2:20" ht="22.5" customHeight="1">
-      <c r="B4" s="50" t="s">
+      <c r="B4" s="62" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="62" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="64" t="s">
+        <v>24</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>25</v>
-      </c>
-      <c r="C4" s="50" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" s="52" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" s="52" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>27</v>
       </c>
       <c r="G4" s="3"/>
       <c r="H4" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="62" t="s">
+        <v>26</v>
+      </c>
+      <c r="J4" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="I4" s="50" t="s">
-        <v>28</v>
-      </c>
-      <c r="J4" s="50" t="s">
+      <c r="L4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="M4" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L4" s="10" t="s">
+      <c r="N4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="M4" s="10" t="s">
+      <c r="O4" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="N4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="O4" s="10" t="s">
-        <v>16</v>
-      </c>
     </row>
     <row r="5" spans="2:20" ht="22.5" customHeight="1">
-      <c r="B5" s="51"/>
-      <c r="C5" s="51"/>
-      <c r="D5" s="52"/>
-      <c r="E5" s="52"/>
+      <c r="B5" s="63"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="64"/>
+      <c r="E5" s="64"/>
       <c r="F5" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H5" s="32"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
       <c r="L5" s="12">
         <v>0.1</v>
       </c>
@@ -1757,15 +2178,15 @@
       </c>
     </row>
     <row r="6" spans="2:20" ht="22.5" customHeight="1" thickBot="1">
-      <c r="B6" s="51"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="50"/>
-      <c r="E6" s="53"/>
+      <c r="B6" s="63"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="65"/>
       <c r="F6" s="48"/>
       <c r="G6" s="48"/>
       <c r="H6" s="32"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="51"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
       <c r="L6" s="12">
         <v>0.15</v>
       </c>
@@ -1784,10 +2205,10 @@
     </row>
     <row r="7" spans="2:20" ht="22.5" customHeight="1" thickBot="1">
       <c r="B7" s="33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C7" s="34" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D7" s="35">
         <v>800000</v>
@@ -1831,10 +2252,10 @@
     </row>
     <row r="8" spans="2:20" ht="22.5" customHeight="1" thickBot="1">
       <c r="B8" s="33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C8" s="34" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="D8" s="35">
         <v>650000</v>
@@ -1878,10 +2299,10 @@
     </row>
     <row r="9" spans="2:20" ht="22.5" customHeight="1" thickBot="1">
       <c r="B9" s="33" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D9" s="35">
         <v>300000</v>
@@ -1923,7 +2344,7 @@
     </row>
     <row r="10" spans="2:20" ht="22.5" customHeight="1" thickBot="1">
       <c r="E10" s="38" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F10" s="49"/>
       <c r="G10" s="49"/>
@@ -1979,7 +2400,7 @@
     <row r="12" spans="2:20" ht="22.5" customHeight="1">
       <c r="H12" s="15"/>
       <c r="I12" s="29" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="J12" s="21">
         <f>J10</f>
@@ -1993,7 +2414,7 @@
       <c r="F13" s="24"/>
       <c r="G13" s="24"/>
       <c r="I13" s="30" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="J13" s="22">
         <f>J10-I10</f>
@@ -2003,7 +2424,7 @@
     </row>
     <row r="14" spans="2:20" ht="22.5" customHeight="1">
       <c r="I14" s="31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="J14" s="23">
         <f>I10</f>
@@ -2013,7 +2434,7 @@
     </row>
     <row r="15" spans="2:20" ht="22.5" customHeight="1">
       <c r="I15" s="31" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="J15" s="16">
         <f>J13/J12</f>
@@ -2022,53 +2443,121 @@
     </row>
     <row r="16" spans="2:20" ht="22.5" customHeight="1">
       <c r="I16" s="11" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="J16" s="21">
         <f>J12*1.1</f>
         <v>1936000.0000000002</v>
       </c>
     </row>
-    <row r="17" ht="22.5" customHeight="1"/>
-    <row r="18" ht="22.5" customHeight="1"/>
-    <row r="19" ht="22.5" customHeight="1"/>
-    <row r="20" ht="22.5" customHeight="1"/>
-    <row r="21" ht="22.5" customHeight="1"/>
-    <row r="22" ht="22.5" customHeight="1"/>
-    <row r="23" ht="22.5" customHeight="1"/>
-    <row r="24" ht="22.5" customHeight="1"/>
-    <row r="25" ht="22.5" customHeight="1"/>
-    <row r="26" ht="22.5" customHeight="1"/>
-    <row r="27" ht="22.5" customHeight="1"/>
-    <row r="28" ht="22.5" customHeight="1"/>
-    <row r="29" ht="22.5" customHeight="1"/>
-    <row r="30" ht="22.5" customHeight="1"/>
-    <row r="31" ht="22.5" customHeight="1"/>
-    <row r="32" ht="22.5" customHeight="1"/>
-    <row r="33" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="34" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="35" spans="14:14" ht="22.5" customHeight="1">
-      <c r="N35" s="1" t="s">
+    <row r="17" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="18" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="19" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="20" spans="3:5" ht="22.5" customHeight="1" thickBot="1">
+      <c r="C20" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>35</v>
+      </c>
+      <c r="E20" s="53" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C21" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E21" s="56" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C22" s="57"/>
+      <c r="D22" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="58" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C23" s="57"/>
+      <c r="D23" s="51" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="58"/>
+    </row>
+    <row r="24" spans="3:5" ht="22.5" customHeight="1" thickBot="1">
+      <c r="C24" s="59"/>
+      <c r="D24" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="E24" s="61"/>
+    </row>
+    <row r="25" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C25" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="E25" s="56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="26" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C26" s="57"/>
+      <c r="D26" s="51" t="s">
+        <v>39</v>
+      </c>
+      <c r="E26" s="58"/>
+    </row>
+    <row r="27" spans="3:5" ht="22.5" customHeight="1" thickBot="1">
+      <c r="C27" s="59"/>
+      <c r="D27" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="E27" s="61"/>
+    </row>
+    <row r="28" spans="3:5" ht="22.5" customHeight="1">
+      <c r="C28" s="54" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="36" spans="14:14" ht="22.5" customHeight="1">
-      <c r="N36" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="37" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="38" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="39" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="40" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="41" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="42" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="43" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="44" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="45" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="46" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="47" spans="14:14" ht="22.5" customHeight="1"/>
-    <row r="48" spans="14:14" ht="22.5" customHeight="1"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="3:5" ht="22.5" customHeight="1" thickBot="1">
+      <c r="C29" s="59"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="61" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="31" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="32" spans="3:5" ht="22.5" customHeight="1"/>
+    <row r="33" ht="22.5" customHeight="1"/>
+    <row r="34" ht="22.5" customHeight="1"/>
+    <row r="35" ht="22.5" customHeight="1"/>
+    <row r="36" ht="22.5" customHeight="1"/>
+    <row r="37" ht="22.5" customHeight="1"/>
+    <row r="38" ht="22.5" customHeight="1"/>
+    <row r="39" ht="22.5" customHeight="1"/>
+    <row r="40" ht="22.5" customHeight="1"/>
+    <row r="41" ht="22.5" customHeight="1"/>
+    <row r="42" ht="22.5" customHeight="1"/>
+    <row r="43" ht="22.5" customHeight="1"/>
+    <row r="44" ht="22.5" customHeight="1"/>
+    <row r="45" ht="22.5" customHeight="1"/>
+    <row r="46" ht="22.5" customHeight="1"/>
+    <row r="47" ht="22.5" customHeight="1"/>
+    <row r="48" ht="22.5" customHeight="1"/>
     <row r="49" ht="22.5" customHeight="1"/>
     <row r="50" ht="22.5" customHeight="1"/>
     <row r="51" ht="22.5" customHeight="1"/>
@@ -2134,7 +2623,193 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1314F6AE-24F8-A74F-9C7B-D81FD267D715}">
+  <dimension ref="B2:B39"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K19" sqref="K19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>
+  <sheetData>
+    <row r="2" spans="2:2">
+      <c r="B2" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="2:2">
+      <c r="B3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="2:2">
+      <c r="B5" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="6" spans="2:2">
+      <c r="B6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="2:2">
+      <c r="B8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="2:2">
+      <c r="B9" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2">
+      <c r="B11" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2">
+      <c r="B12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="2:2">
+      <c r="B13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="2:2">
+      <c r="B16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2">
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2">
+      <c r="B18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2">
+      <c r="B19" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2">
+      <c r="B20" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2">
+      <c r="B21" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
+      <c r="B22" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2">
+      <c r="B24" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2">
+      <c r="B25" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2">
+      <c r="B26" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2">
+      <c r="B27" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2">
+      <c r="B29" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2">
+      <c r="B30" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2">
+      <c r="B31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
+      <c r="B32" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2">
+      <c r="B33" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="34" spans="2:2">
+      <c r="B34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="36" spans="2:2">
+      <c r="B36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
+      <c r="B37" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="38" spans="2:2">
+      <c r="B38" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="39" spans="2:2">
+      <c r="B39" t="s">
+        <v>76</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101006632764D35F10A4D8B5BB0A810B77478" ma:contentTypeVersion="0" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="3e6e98fca06f93bbe2242eb56a6cb1cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="c889ecaaa051264ff38733239b316710">
     <xsd:element name="properties">
@@ -2248,32 +2923,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3E80F4-BD31-45CA-8169-0725B6ADD5A2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF20DB80-65FB-4557-92A9-B01A20B8573A}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
@@ -2288,9 +2941,16 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF20DB80-65FB-4557-92A9-B01A20B8573A}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A3E80F4-BD31-45CA-8169-0725B6ADD5A2}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>

</xml_diff>